<commit_message>
more work on SRDP
</commit_message>
<xml_diff>
--- a/doc/SRDP.xlsx
+++ b/doc/SRDP.xlsx
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>The URI of the electronic datasheet (EDS) of the device.</t>
-  </si>
-  <si>
-    <t>&lt;64k octets</t>
   </si>
   <si>
     <t>/device/1/id</t>
@@ -396,6 +393,9 @@
   </si>
   <si>
     <t>Field*</t>
+  </si>
+  <si>
+    <t>&lt; (64k - 12) octets</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1165,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1233,16 +1233,16 @@
         <v>16</v>
       </c>
       <c r="K3" s="39" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="25.5" customHeight="1" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="37" t="s">
         <v>5</v>
@@ -1251,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="40" t="s">
         <v>3</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="6" spans="1:11" s="26" customFormat="1" ht="13.5" customHeight="1">
       <c r="A6" s="67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="46"/>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="64">
         <v>0</v>
@@ -1370,7 +1370,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="48" t="s">
         <v>11</v>
@@ -1404,7 +1404,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="48" t="s">
         <v>11</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="12" spans="1:11" s="8" customFormat="1" ht="34.5" customHeight="1">
       <c r="A12" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="57">
@@ -1437,7 +1437,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="48" t="s">
         <v>11</v>
@@ -1483,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" s="47" t="s">
         <v>11</v>
@@ -1516,7 +1516,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="47" t="s">
         <v>11</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="16" spans="1:11" s="20" customFormat="1" ht="34.5" customHeight="1">
       <c r="A16" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="56">
@@ -1550,7 +1550,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G16" s="47" t="s">
         <v>11</v>
@@ -1596,7 +1596,7 @@
         <v>10</v>
       </c>
       <c r="F18" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="48" t="s">
         <v>11</v>
@@ -1629,7 +1629,7 @@
         <v>10</v>
       </c>
       <c r="F19" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19" s="48" t="s">
         <v>11</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="20" spans="1:11" s="8" customFormat="1" ht="34.5" customHeight="1">
       <c r="A20" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="32"/>
       <c r="C20" s="57">
@@ -1663,7 +1663,7 @@
         <v>10</v>
       </c>
       <c r="F20" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="48" t="s">
         <v>11</v>
@@ -1755,12 +1755,12 @@
   <sheetData>
     <row r="1" spans="2:9" ht="33.75" customHeight="1">
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
       <c r="B2" s="66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="27.75" customHeight="1">
@@ -1789,7 +1789,7 @@
         <v>40</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:9" s="20" customFormat="1" ht="33.75" customHeight="1">
@@ -1807,10 +1807,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:9" s="8" customFormat="1" ht="33.75" customHeight="1">
@@ -1857,7 +1857,7 @@
     </row>
     <row r="8" spans="2:9" s="8" customFormat="1" ht="33.75" customHeight="1">
       <c r="B8" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="14">
         <v>1</v>
@@ -1869,10 +1869,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:9" s="20" customFormat="1" ht="33.75" customHeight="1">
@@ -1897,7 +1897,7 @@
     </row>
     <row r="10" spans="2:9" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="B10" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="14">
         <v>1</v>
@@ -1906,19 +1906,19 @@
         <v>1024</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:9" s="23" customFormat="1" ht="33.75" customHeight="1">
       <c r="B11" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="19">
         <v>1</v>
@@ -1927,19 +1927,19 @@
         <v>1025</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="2:9" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="B12" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="14">
         <v>1</v>
@@ -1948,19 +1948,19 @@
         <v>1026</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:9" s="23" customFormat="1" ht="33.75" customHeight="1">
       <c r="B13" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="19">
         <v>1</v>
@@ -1972,16 +1972,16 @@
         <v>8</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="2:9" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="B14" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="14">
         <v>1</v>
@@ -1993,16 +1993,16 @@
         <v>50</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="2:9" s="23" customFormat="1" ht="33.75" customHeight="1">
       <c r="B15" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="19">
         <v>1</v>
@@ -2014,16 +2014,16 @@
         <v>8</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="2:9" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="B16" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="14">
         <v>1</v>
@@ -2035,16 +2035,16 @@
         <v>50</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="2:8" s="23" customFormat="1" ht="33.75" customHeight="1">
       <c r="B17" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="19">
         <v>1</v>
@@ -2056,16 +2056,16 @@
         <v>8</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:8" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="B18" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="14">
         <v>1</v>
@@ -2077,16 +2077,16 @@
         <v>50</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:8" s="23" customFormat="1" ht="33.75" customHeight="1">
       <c r="B19" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="19">
         <v>1</v>
@@ -2098,16 +2098,16 @@
         <v>50</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="2:8" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="B20" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="14">
         <v>1</v>
@@ -2119,16 +2119,16 @@
         <v>50</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="23" customFormat="1" ht="33.75" customHeight="1">
       <c r="B21" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" s="19">
         <v>1</v>
@@ -2140,16 +2140,16 @@
         <v>8</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:8" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="B22" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22" s="14">
         <v>1</v>
@@ -2161,16 +2161,16 @@
         <v>50</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="2:8" s="23" customFormat="1" ht="33.75" customHeight="1">
       <c r="B23" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C23" s="19">
         <v>1</v>
@@ -2182,16 +2182,16 @@
         <v>50</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:8" s="17" customFormat="1" ht="33.75" customHeight="1">
       <c r="B24" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" s="14">
         <v>1</v>
@@ -2203,11 +2203,11 @@
         <v>50</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2272,7 +2272,7 @@
         <v>40</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="20" customFormat="1" ht="33.75" customHeight="1">
@@ -2290,10 +2290,10 @@
         <v>8</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:9" s="8" customFormat="1" ht="33.75" customHeight="1">
@@ -2337,12 +2337,12 @@
         <v>54</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:9" s="8" customFormat="1" ht="33.75" customHeight="1">
       <c r="B7" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="14">
         <v>1</v>
@@ -2354,10 +2354,10 @@
         <v>8</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:9" s="20" customFormat="1" ht="33.75" customHeight="1">

</xml_diff>

<commit_message>
work on Python SRDP frame receiver
</commit_message>
<xml_diff>
--- a/doc/SRDP.xlsx
+++ b/doc/SRDP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="11580" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="11580" windowHeight="5370"/>
   </bookViews>
   <sheets>
     <sheet name="Frame Format" sheetId="3" r:id="rId1"/>
@@ -414,7 +414,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,6 +502,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -706,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -860,12 +868,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -877,6 +879,42 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1176,8 +1214,8 @@
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1294,7 +1332,7 @@
       <c r="K5" s="49"/>
     </row>
     <row r="6" spans="1:11" s="26" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="65" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="25"/>
@@ -1320,36 +1358,36 @@
       <c r="J7" s="46"/>
       <c r="K7" s="50"/>
     </row>
-    <row r="8" spans="1:11" s="65" customFormat="1" ht="34.5" customHeight="1" thickTop="1">
+    <row r="8" spans="1:11" s="63" customFormat="1" ht="34.5" customHeight="1" thickTop="1">
       <c r="A8" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="59"/>
-      <c r="C8" s="61">
-        <v>1</v>
-      </c>
-      <c r="D8" s="62">
-        <v>1</v>
-      </c>
-      <c r="E8" s="63">
+      <c r="C8" s="76">
+        <v>1</v>
+      </c>
+      <c r="D8" s="77">
+        <v>0</v>
+      </c>
+      <c r="E8" s="61">
         <v>0</v>
       </c>
       <c r="F8" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="64">
+      <c r="G8" s="62">
         <v>0</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="64" t="s">
+      <c r="J8" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="60" t="str">
+      <c r="K8" s="70" t="str">
         <f>"-"</f>
         <v>-</v>
       </c>
@@ -1372,11 +1410,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="32"/>
-      <c r="C10" s="57">
-        <v>1</v>
-      </c>
-      <c r="D10" s="44">
-        <v>2</v>
+      <c r="C10" s="74">
+        <v>1</v>
+      </c>
+      <c r="D10" s="75">
+        <v>1</v>
       </c>
       <c r="E10" s="43" t="s">
         <v>10</v>
@@ -1390,13 +1428,13 @@
       <c r="H10" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="68" t="s">
         <v>13</v>
       </c>
       <c r="J10" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="52" t="str">
+      <c r="K10" s="69" t="str">
         <f>"-"</f>
         <v>-</v>
       </c>
@@ -1410,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="43" t="s">
         <v>10</v>
@@ -1443,7 +1481,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="43" t="s">
         <v>10</v>
@@ -1489,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="42" t="s">
         <v>10</v>
@@ -1518,11 +1556,11 @@
         <v>18</v>
       </c>
       <c r="B15" s="28"/>
-      <c r="C15" s="56">
+      <c r="C15" s="72">
         <v>2</v>
       </c>
-      <c r="D15" s="41">
-        <v>3</v>
+      <c r="D15" s="73">
+        <v>2</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>10</v>
@@ -1536,13 +1574,13 @@
       <c r="H15" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="47" t="s">
+      <c r="I15" s="66" t="s">
         <v>28</v>
       </c>
       <c r="J15" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="51" t="str">
+      <c r="K15" s="67" t="str">
         <f>"-"</f>
         <v>-</v>
       </c>
@@ -1556,7 +1594,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>10</v>
@@ -1602,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" s="43" t="s">
         <v>10</v>
@@ -1635,7 +1673,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="43" t="s">
         <v>10</v>
@@ -1669,7 +1707,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="43" t="s">
         <v>10</v>
@@ -1746,7 +1784,7 @@
   </sheetPr>
   <dimension ref="B1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1771,12 +1809,12 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="27.75" customHeight="1">
-      <c r="B3" s="66"/>
+      <c r="B3" s="64"/>
     </row>
     <row r="4" spans="2:9" s="9" customFormat="1" ht="33.75" customHeight="1">
       <c r="B4" s="9" t="s">

</xml_diff>